<commit_message>
massive reeds update from Jonathan
Starting at 2010 not 2009, so all indexes for 2030, 2040, 2050  is now 20, 30, 40
</commit_message>
<xml_diff>
--- a/PV_ICE/baselines/LiteratureProjections/NREL_Energy_Futures_2021.xlsx
+++ b/PV_ICE/baselines/LiteratureProjections/NREL_Energy_Futures_2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sayala\Documents\GitHub\CircularEconomy-MassFlowCalculator\PV_ICE\baselines\LiteratureProjections\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC24264E-4140-4636-AD0B-EE908335423B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B24BDEA1-1F2D-4EB0-BE53-110149C68A88}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{AF72BD23-974C-4E35-956F-C0D9DFB4E55E}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
   <si>
     <t>Rooftop PV_GW</t>
   </si>
@@ -56,9 +56,6 @@
   </si>
   <si>
     <t>High Electrification [MW]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NEW INSTALLS PV </t>
   </si>
   <si>
     <t>AC to DC Ratio</t>
@@ -85,15 +82,6 @@
     <t>PV ICE module baseline</t>
   </si>
   <si>
-    <t>PV ICE</t>
-  </si>
-  <si>
-    <t>EF</t>
-  </si>
-  <si>
-    <t>SFS</t>
-  </si>
-  <si>
     <t>SFS Reference.Mod</t>
   </si>
   <si>
@@ -106,20 +94,38 @@
     <t>MW Cumulative Installs to 2018 (initial value)</t>
   </si>
   <si>
-    <t>Copy Paste multiply by 1000 (to MW) and by 0.85 starting 2020 (market Share silicon), and Sort Columsn F, G, J, K (and years A, I)</t>
-  </si>
-  <si>
     <t>USED IN 2021 EF BAseline</t>
   </si>
   <si>
     <t>Comparison from Rawish data</t>
+  </si>
+  <si>
+    <t>COPY PASTE</t>
+  </si>
+  <si>
+    <t>OFF YEARS</t>
+  </si>
+  <si>
+    <t>NEW INSTALLS PV, considering Market Share</t>
+  </si>
+  <si>
+    <t>New Installs with AC DC RAtio</t>
+  </si>
+  <si>
+    <t>PV ICE [MW]</t>
+  </si>
+  <si>
+    <t>EF  [MW]</t>
+  </si>
+  <si>
+    <t>SFS  [MW]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -164,8 +170,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -187,8 +215,30 @@
         <fgColor rgb="FFFFCC99"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -341,16 +391,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -361,12 +427,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
@@ -387,16 +447,40 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -406,12 +490,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="14" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="6">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Good" xfId="4" builtinId="26"/>
     <cellStyle name="Input" xfId="3" builtinId="20"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="5" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -452,11 +544,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'new installs PV'!$X$3</c:f>
+              <c:f>'new installs PV'!$AB$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>PV ICE</c:v>
+                  <c:v>PV ICE [MW]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -471,186 +563,9 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:numRef>
-              <c:f>'new installs PV'!$W$4:$W$59</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="56"/>
-                <c:pt idx="0">
-                  <c:v>1995</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1996</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1997</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1998</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1999</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2001</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2002</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2003</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2004</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2005</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2006</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2007</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>2008</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>2009</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>2010</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>2011</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>2012</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>2013</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>2014</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>2015</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>2016</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>2017</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>2018</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>2019</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>2020</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>2021</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>2022</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>2023</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>2024</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>2025</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>2026</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>2027</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>2028</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>2029</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>2030</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>2031</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>2032</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>2033</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>2034</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>2035</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>2036</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>2037</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>2038</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>2039</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>2040</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>2041</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>2042</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>2043</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>2044</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>2045</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>2046</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>2047</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>2048</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>2049</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>2050</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'new installs PV'!$X$4:$X$59</c:f>
+              <c:f>'new installs PV'!$AB$4:$AB$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="56"/>
@@ -827,404 +742,20 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-AFC5-46BB-806A-8C25E0E46A40}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'new installs PV'!$Y$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>EF</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:numRef>
-              <c:f>'new installs PV'!$W$4:$W$59</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="56"/>
-                <c:pt idx="0">
-                  <c:v>1995</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1996</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1997</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1998</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1999</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2001</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2002</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2003</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2004</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2005</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2006</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2007</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>2008</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>2009</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>2010</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>2011</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>2012</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>2013</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>2014</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>2015</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>2016</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>2017</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>2018</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>2019</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>2020</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>2021</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>2022</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>2023</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>2024</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>2025</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>2026</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>2027</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>2028</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>2029</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>2030</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>2031</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>2032</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>2033</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>2034</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>2035</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>2036</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>2037</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>2038</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>2039</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>2040</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>2041</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>2042</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>2043</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>2044</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>2045</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>2046</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>2047</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>2048</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>2049</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>2050</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'new installs PV'!$Y$4:$Y$59</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="56"/>
-                <c:pt idx="0">
-                  <c:v>12.5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>9.6676666670000007</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>11.622</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>11.781000000000001</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16.884666670000001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>20.926666669999999</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>27.984999999999999</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>42.475999999999999</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>59.744999999999997</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>94.751999999999995</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>96.581173219999997</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>98.21307161</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>324.23274839999999</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>314.58510869999998</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>431.24480390000002</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>719.84443759999999</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1781.377078</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>3064.1622809999999</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>4037.4491130000001</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>3722.1994850000001</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>6834.3288130000001</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>12897.665950000001</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>9784.5062149999994</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>9352.5294479999993</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>10949.78234</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>14454.770399725652</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>29515.260985639161</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>29515.260985639161</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>18890.512643677579</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>18890.512643677579</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>16238.879778072385</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>16238.879778072385</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>31283.159548301846</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>31283.159548301846</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>43951.271441554672</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>43951.271441554672</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>48105.30432171448</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>48105.30432171448</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>32257.627384008374</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>32257.627384008374</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>20055.842856203435</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>20055.842856203435</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>19293.698106263313</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>19293.698106263313</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>50646.427669738965</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>50646.427669738965</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>19860.369071007961</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>19860.369071007961</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>39937.784018518752</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>39937.784018518752</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>32400.914343086391</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>32400.914343086391</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>44431.939714859429</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>44431.939714859429</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>62577.899925893202</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>62577.899925893202</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-AFC5-46BB-806A-8C25E0E46A40}"/>
+              <c16:uniqueId val="{00000001-3FE8-43CD-A635-0D1C99AC8110}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'new installs PV'!$Z$3</c:f>
+              <c:f>'new installs PV'!$AD$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>SFS</c:v>
+                  <c:v>SFS  [MW]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1241,7 +772,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'new installs PV'!$W$4:$W$59</c:f>
+              <c:f>'new installs PV'!$AA$4:$AA$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="56"/>
@@ -1418,7 +949,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'new installs PV'!$Z$4:$Z$59</c:f>
+              <c:f>'new installs PV'!$AD$4:$AD$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="56"/>
@@ -1596,6 +1127,213 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-AFC5-46BB-806A-8C25E0E46A40}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'new installs PV'!$AC$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>EF  [MW]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'new installs PV'!$AC$4:$AC$59</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="56"/>
+                <c:pt idx="0">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.6676666670000007</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.622</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.781000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.884666670000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20.926666669999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>27.984999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>42.475999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>59.744999999999997</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>94.751999999999995</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>96.581173219999997</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>98.21307161</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>324.23274839999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>314.58510869999998</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>431.24480390000002</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>719.84443759999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1781.377078</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3064.1622809999999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4037.4491130000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3722.1994850000001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>6834.3288130000001</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>12897.665950000001</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>9784.5062149999994</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9352.5294479999993</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>10949.78234</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>14454.770399725652</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>29515.260985639161</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>29515.260985639161</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>18890.512643677579</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>18890.512643677579</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>16238.879778072385</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>16238.879778072385</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>31283.159548301846</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>31283.159548301846</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>43951.271441554672</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>43951.271441554672</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>48105.30432171448</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>48105.30432171448</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>32257.627384008374</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>32257.627384008374</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>20055.842856203435</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>20055.842856203435</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>19293.698106263313</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>19293.698106263313</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>50646.427669738965</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>50646.427669738965</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>19860.369071007961</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>19860.369071007961</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>39937.784018518752</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>39937.784018518752</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>32400.914343086391</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>32400.914343086391</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>44431.939714859429</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>44431.939714859429</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>62577.899925893202</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>62577.899925893202</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-3FE8-43CD-A635-0D1C99AC8110}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2439,13 +2177,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>26</xdr:col>
+      <xdr:col>30</xdr:col>
       <xdr:colOff>209549</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>376237</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>41</xdr:col>
+      <xdr:col>45</xdr:col>
       <xdr:colOff>295274</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>185737</xdr:rowOff>
@@ -2791,27 +2529,27 @@
       <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2825,10 +2563,10 @@
       <c r="C3">
         <v>41.076723385145499</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>16.795572727272699</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="1">
         <v>37.128700161271297</v>
       </c>
     </row>
@@ -2842,10 +2580,10 @@
       <c r="C4">
         <v>51.268514335123498</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>20.908446363636401</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="1">
         <v>62.7384416488865</v>
       </c>
     </row>
@@ -2859,10 +2597,10 @@
       <c r="C5">
         <v>75.015006991810495</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>25.792741818181799</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="1">
         <v>99.616469391052505</v>
       </c>
     </row>
@@ -2876,10 +2614,10 @@
       <c r="C6">
         <v>89.475100470251704</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <v>30.935123636363599</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="1">
         <v>134.733147399925</v>
       </c>
     </row>
@@ -2893,10 +2631,10 @@
       <c r="C7">
         <v>100.957003120091</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="1">
         <v>37.526330000000002</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="1">
         <v>161.821145189253</v>
       </c>
     </row>
@@ -2910,10 +2648,10 @@
       <c r="C8">
         <v>125.235676285975</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="1">
         <v>45.875010909090904</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="1">
         <v>207.33235988875199</v>
       </c>
     </row>
@@ -2927,10 +2665,10 @@
       <c r="C9">
         <v>160.19696564484801</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="1">
         <v>56.131709999999998</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="1">
         <v>290.50558331976799</v>
       </c>
     </row>
@@ -2944,10 +2682,10 @@
       <c r="C10">
         <v>198.954028469929</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="1">
         <v>67.492456363636407</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="1">
         <v>403.33153664398401</v>
       </c>
     </row>
@@ -2961,10 +2699,10 @@
       <c r="C11">
         <v>223.42721913419001</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="1">
         <v>80.480386363636399</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="1">
         <v>485.16087153802999</v>
       </c>
     </row>
@@ -2978,10 +2716,10 @@
       <c r="C12">
         <v>236.84451085926099</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="1">
         <v>95.322164545454498</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="1">
         <v>524.56542997676604</v>
       </c>
     </row>
@@ -2995,10 +2733,10 @@
       <c r="C13">
         <v>248.95698882873</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="1">
         <v>111.444223636364</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="1">
         <v>582.11597042682502</v>
       </c>
     </row>
@@ -3012,10 +2750,10 @@
       <c r="C14">
         <v>289.64260309998701</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="1">
         <v>127.604308181818</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="1">
         <v>593.87906054333405</v>
       </c>
     </row>
@@ -3029,10 +2767,10 @@
       <c r="C15">
         <v>303.58594854886297</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="1">
         <v>139.236943636364</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="1">
         <v>639.29218521486405</v>
       </c>
     </row>
@@ -3046,10 +2784,10 @@
       <c r="C16">
         <v>336.10154720815598</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="1">
         <v>148.088826363636</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="1">
         <v>682.98325261898503</v>
       </c>
     </row>
@@ -3063,10 +2801,10 @@
       <c r="C17">
         <v>361.99709317474998</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="1">
         <v>155.33214272727301</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="1">
         <v>741.40792082883002</v>
       </c>
     </row>
@@ -3080,10 +2818,10 @@
       <c r="C18">
         <v>399.13920644611602</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="1">
         <v>161.52204727272701</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18" s="1">
         <v>823.134117188196</v>
       </c>
     </row>
@@ -3097,10 +2835,10 @@
       <c r="C19">
         <v>452.97766085868898</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="1">
         <v>167.21188818181801</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E19" s="1">
         <v>907.75283817318802</v>
       </c>
     </row>
@@ -3111,24 +2849,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7755643-5611-467E-B7A2-2A0E07DAA24D}">
-  <dimension ref="A1:Z59"/>
+  <dimension ref="A1:AD59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="T5" sqref="T5"/>
+    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="AL20" sqref="AL20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="17" max="17" width="19.28515625" customWidth="1"/>
-    <col min="19" max="19" width="26" customWidth="1"/>
-    <col min="20" max="20" width="13.5703125" customWidth="1"/>
-    <col min="21" max="21" width="24.140625" customWidth="1"/>
+    <col min="20" max="20" width="17.42578125" customWidth="1"/>
+    <col min="21" max="21" width="19.28515625" customWidth="1"/>
+    <col min="23" max="23" width="26" customWidth="1"/>
+    <col min="24" max="24" width="13.5703125" customWidth="1"/>
+    <col min="25" max="25" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1">
         <v>1.1000000000000001</v>
@@ -3136,87 +2875,103 @@
       <c r="C1">
         <v>1.3</v>
       </c>
-      <c r="N1" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-    </row>
-    <row r="2" spans="1:26" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:30" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="O2" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="P2" s="8"/>
-    </row>
-    <row r="3" spans="1:26" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="F2" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="31"/>
+      <c r="I2" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="M2" s="37" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2" s="37"/>
+      <c r="O2" s="37"/>
+      <c r="S2" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="T2" s="32"/>
+    </row>
+    <row r="3" spans="1:30" s="29" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="I3" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J3" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N3" t="s">
+      <c r="L3" s="30"/>
+      <c r="N3" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="O3" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="R3" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="S3" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="T3" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="S3" s="1" t="s">
+      <c r="W3" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB3" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="X3" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="Y3" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="Z3" s="23" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+      <c r="AC3" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD3" s="27" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" ht="30" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2018</v>
       </c>
@@ -3226,56 +2981,67 @@
       <c r="C4">
         <v>41.076723385145499</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>16.795572727272699</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="1">
         <v>37.128700161271297</v>
       </c>
       <c r="F4">
-        <f>B4+C4</f>
-        <v>57.335402476054597</v>
+        <f>B4*B1+C4*C1</f>
+        <v>71.284287400689152</v>
       </c>
       <c r="G4">
         <f>D4*$B$1+E4*$C$1</f>
         <v>66.742440209652656</v>
       </c>
-      <c r="N4" s="5">
+      <c r="M4">
         <v>2018</v>
       </c>
-      <c r="O4" s="5">
-        <v>57335.402476054594</v>
-      </c>
-      <c r="P4" s="5">
-        <v>66742.440209652661</v>
-      </c>
-      <c r="Q4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="S4" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="T4" s="12">
-        <f>SUM(X4:X27)</f>
+      <c r="N4">
+        <v>71.284287400689152</v>
+      </c>
+      <c r="O4">
+        <v>66.742440209652656</v>
+      </c>
+      <c r="R4" s="4">
+        <v>2018</v>
+      </c>
+      <c r="S4" s="4">
+        <f>N4*0.85*1000</f>
+        <v>60591.644290585777</v>
+      </c>
+      <c r="T4" s="4">
+        <f>O4*0.85*1000</f>
+        <v>56731.074178204755</v>
+      </c>
+      <c r="U4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="W4" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="X4" s="9">
+        <f>SUM(AB4:AB27)</f>
         <v>53767.259726437005</v>
       </c>
-      <c r="U4" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="W4">
+      <c r="Y4" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA4">
         <v>1995</v>
       </c>
-      <c r="X4" s="21">
+      <c r="AB4" s="18">
         <v>12.5</v>
       </c>
-      <c r="Y4" s="21">
+      <c r="AC4" s="18">
         <v>12.5</v>
       </c>
-      <c r="Z4" s="21">
+      <c r="AD4" s="18">
         <v>12.5</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:30" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2020</v>
       </c>
@@ -3285,10 +3051,10 @@
       <c r="C5">
         <v>51.268514335123498</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>20.908446363636401</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="1">
         <v>62.7384416488865</v>
       </c>
       <c r="F5">
@@ -3311,41 +3077,52 @@
         <f>G5</f>
         <v>37.816824933899838</v>
       </c>
-      <c r="N5" s="9">
+      <c r="M5">
         <v>2019</v>
       </c>
-      <c r="O5" s="24">
-        <v>17005.612234971355</v>
-      </c>
-      <c r="P5" s="24">
-        <v>37816.824933899836</v>
-      </c>
-      <c r="Q5" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="S5" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="T5" s="15">
+      <c r="N5">
+        <v>17.005612234971355</v>
+      </c>
+      <c r="O5">
+        <v>37.816824933899838</v>
+      </c>
+      <c r="R5" s="6">
+        <v>2019</v>
+      </c>
+      <c r="S5" s="6">
+        <f>N5*0.85*1000</f>
+        <v>14454.770399725652</v>
+      </c>
+      <c r="T5" s="6">
+        <f t="shared" ref="T5:T7" si="0">O5*0.85*1000</f>
+        <v>32144.301193814863</v>
+      </c>
+      <c r="U5" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="W5" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="X5" s="12">
         <v>57335.402476054602</v>
       </c>
-      <c r="U5" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="W5">
+      <c r="Y5" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA5">
         <v>1996</v>
       </c>
-      <c r="X5" s="21">
+      <c r="AB5" s="18">
         <v>9.6676666670000007</v>
       </c>
-      <c r="Y5" s="21">
+      <c r="AC5" s="18">
         <v>9.6676666670000007</v>
       </c>
-      <c r="Z5" s="21">
+      <c r="AD5" s="18">
         <v>9.6676666670000007</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" ht="30" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2022</v>
       </c>
@@ -3355,68 +3132,79 @@
       <c r="C6">
         <v>75.015006991810495</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <v>25.792741818181799</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="1">
         <v>99.616469391052505</v>
       </c>
       <c r="F6">
-        <f t="shared" ref="F6:F20" si="0">(B6-B5)*$B$1+(C6-C5)*$C$1</f>
+        <f t="shared" ref="F6:F20" si="1">(B6-B5)*$B$1+(C6-C5)*$C$1</f>
         <v>34.723836453693131</v>
       </c>
       <c r="G6">
-        <f t="shared" ref="G6:G20" si="1">(D6-D5)*$B$1+(E6-E5)*$C$1</f>
+        <f t="shared" ref="G6:G20" si="2">(D6-D5)*$B$1+(E6-E5)*$C$1</f>
         <v>53.31416106481575</v>
       </c>
       <c r="I6">
-        <f t="shared" ref="I6:I20" si="2">A6-1</f>
+        <f t="shared" ref="I6:I20" si="3">A6-1</f>
         <v>2021</v>
       </c>
       <c r="J6">
-        <f t="shared" ref="J6:J20" si="3">F6</f>
+        <f t="shared" ref="J6:J20" si="4">F6</f>
         <v>34.723836453693131</v>
       </c>
       <c r="K6">
-        <f t="shared" ref="K6:K20" si="4">G6</f>
+        <f t="shared" ref="K6:K20" si="5">G6</f>
         <v>53.31416106481575</v>
       </c>
+      <c r="M6">
+        <v>2020</v>
+      </c>
       <c r="N6">
+        <v>17.005612234971355</v>
+      </c>
+      <c r="O6">
+        <v>37.816824933899838</v>
+      </c>
+      <c r="R6">
         <v>2020</v>
       </c>
-      <c r="O6" s="11">
+      <c r="S6" s="11">
+        <f>N6*0.85*1000</f>
         <v>14454.770399725652</v>
       </c>
-      <c r="P6" s="25">
-        <v>32144.301193814859</v>
-      </c>
-      <c r="Q6" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="S6" s="14" t="s">
+      <c r="T6" s="20">
+        <f t="shared" si="0"/>
+        <v>32144.301193814863</v>
+      </c>
+      <c r="U6" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="T6" s="15">
-        <f>SUM(T9,Z20:Z27)</f>
+      <c r="W6" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="X6" s="12">
+        <f>SUM(X9,AD20:AD27)</f>
         <v>53783.95990052999</v>
       </c>
-      <c r="U6" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="W6">
+      <c r="Y6" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA6">
         <v>1997</v>
       </c>
-      <c r="X6" s="21">
+      <c r="AB6" s="18">
         <v>11.622</v>
       </c>
-      <c r="Y6" s="21">
+      <c r="AC6" s="18">
         <v>11.622</v>
       </c>
-      <c r="Z6" s="21">
+      <c r="AD6" s="18">
         <v>11.622</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2024</v>
       </c>
@@ -3426,59 +3214,70 @@
       <c r="C7">
         <v>89.475100470251704</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="1">
         <v>30.935123636363599</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="1">
         <v>134.733147399925</v>
       </c>
       <c r="F7">
+        <f t="shared" si="1"/>
+        <v>22.224132521973623</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="2"/>
+        <v>51.308301411534231</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="3"/>
+        <v>2023</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="4"/>
+        <v>22.224132521973623</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="5"/>
+        <v>51.308301411534231</v>
+      </c>
+      <c r="M7">
+        <v>2021</v>
+      </c>
+      <c r="N7">
+        <v>34.723836453693131</v>
+      </c>
+      <c r="O7">
+        <v>53.31416106481575</v>
+      </c>
+      <c r="R7">
+        <v>2021</v>
+      </c>
+      <c r="S7" s="11">
+        <f>N7*0.85*1000</f>
+        <v>29515.260985639161</v>
+      </c>
+      <c r="T7" s="20">
         <f t="shared" si="0"/>
-        <v>22.224132521973623</v>
-      </c>
-      <c r="G7">
-        <f t="shared" si="1"/>
-        <v>51.308301411534231</v>
-      </c>
-      <c r="I7">
-        <f t="shared" si="2"/>
-        <v>2023</v>
-      </c>
-      <c r="J7">
-        <f t="shared" si="3"/>
-        <v>22.224132521973623</v>
-      </c>
-      <c r="K7">
-        <f t="shared" si="4"/>
-        <v>51.308301411534231</v>
-      </c>
-      <c r="N7">
-        <v>2021</v>
-      </c>
-      <c r="O7" s="14">
-        <v>29515.260985639161</v>
-      </c>
-      <c r="P7" s="26">
         <v>45317.036905093388</v>
       </c>
-      <c r="Q7" s="29"/>
-      <c r="S7" s="14"/>
-      <c r="T7" s="17"/>
-      <c r="U7" s="16"/>
-      <c r="W7">
+      <c r="U7" s="34"/>
+      <c r="W7" s="11"/>
+      <c r="X7" s="14"/>
+      <c r="Y7" s="13"/>
+      <c r="AA7">
         <v>1998</v>
       </c>
-      <c r="X7" s="21">
+      <c r="AB7" s="18">
         <v>11.781000000000001</v>
       </c>
-      <c r="Y7" s="21">
+      <c r="AC7" s="18">
         <v>11.781000000000001</v>
       </c>
-      <c r="Z7" s="21">
+      <c r="AD7" s="18">
         <v>11.781000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" ht="30" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2026</v>
       </c>
@@ -3488,66 +3287,77 @@
       <c r="C8">
         <v>100.957003120091</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="1">
         <v>37.526330000000002</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="1">
         <v>161.821145189253</v>
       </c>
       <c r="F8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>19.104564444791041</v>
       </c>
       <c r="G8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>42.464724126126441</v>
       </c>
       <c r="I8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2025</v>
       </c>
       <c r="J8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>19.104564444791041</v>
       </c>
       <c r="K8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>42.464724126126441</v>
       </c>
+      <c r="M8">
+        <v>2022</v>
+      </c>
       <c r="N8">
+        <v>34.723836453693131</v>
+      </c>
+      <c r="O8">
+        <v>53.31416106481575</v>
+      </c>
+      <c r="R8">
         <v>2022</v>
       </c>
-      <c r="O8" s="14">
+      <c r="S8" s="11">
+        <f t="shared" ref="S8:S36" si="6">N8*0.85*1000</f>
         <v>29515.260985639161</v>
       </c>
-      <c r="P8" s="26">
+      <c r="T8" s="20">
+        <f t="shared" ref="T8:T36" si="7">O8*0.85*1000</f>
         <v>45317.036905093388</v>
       </c>
-      <c r="Q8" s="29"/>
-      <c r="S8" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="T8" s="15">
-        <f>SUM(X4:X19)</f>
+      <c r="U8" s="34"/>
+      <c r="W8" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="X8" s="12">
+        <f>SUM(AB4:AB19)</f>
         <v>2293.0413434370003</v>
       </c>
-      <c r="U8" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="W8">
+      <c r="Y8" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA8">
         <v>1999</v>
       </c>
-      <c r="X8" s="21">
+      <c r="AB8" s="18">
         <v>16.884666670000001</v>
       </c>
-      <c r="Y8" s="21">
+      <c r="AC8" s="18">
         <v>16.884666670000001</v>
       </c>
-      <c r="Z8" s="21">
+      <c r="AD8" s="18">
         <v>16.884666670000001</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:30" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2028</v>
       </c>
@@ -3557,65 +3367,76 @@
       <c r="C9">
         <v>125.235676285975</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="1">
         <v>45.875010909090904</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="1">
         <v>207.33235988875199</v>
       </c>
       <c r="F9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>36.803717115649235</v>
       </c>
       <c r="G9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>68.348128109348693</v>
       </c>
       <c r="I9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2027</v>
       </c>
       <c r="J9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>36.803717115649235</v>
       </c>
       <c r="K9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>68.348128109348693</v>
       </c>
+      <c r="M9">
+        <v>2023</v>
+      </c>
       <c r="N9">
+        <v>22.224132521973623</v>
+      </c>
+      <c r="O9">
+        <v>51.308301411534231</v>
+      </c>
+      <c r="R9">
         <v>2023</v>
       </c>
-      <c r="O9" s="14">
+      <c r="S9" s="11">
+        <f t="shared" si="6"/>
         <v>18890.512643677579</v>
       </c>
-      <c r="P9" s="26">
+      <c r="T9" s="20">
+        <f t="shared" si="7"/>
         <v>43612.056199804094</v>
       </c>
-      <c r="Q9" s="29"/>
-      <c r="S9" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="T9" s="19">
+      <c r="U9" s="34"/>
+      <c r="W9" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="X9" s="16">
         <v>1200.6513499999901</v>
       </c>
-      <c r="U9" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="W9">
+      <c r="Y9" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA9">
         <v>2000</v>
       </c>
-      <c r="X9" s="21">
+      <c r="AB9" s="18">
         <v>20.926666669999999</v>
       </c>
-      <c r="Y9" s="21">
+      <c r="AC9" s="18">
         <v>20.926666669999999</v>
       </c>
-      <c r="Z9" s="21">
+      <c r="AD9" s="18">
         <v>20.926666669999999</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2030</v>
       </c>
@@ -3625,56 +3446,67 @@
       <c r="C10">
         <v>160.19696564484801</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="1">
         <v>56.131709999999998</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="1">
         <v>290.50558331976799</v>
       </c>
       <c r="F10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>51.707378166534909</v>
       </c>
       <c r="G10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>119.4075594603208</v>
       </c>
       <c r="I10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2029</v>
       </c>
       <c r="J10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>51.707378166534909</v>
       </c>
       <c r="K10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>119.4075594603208</v>
       </c>
+      <c r="M10">
+        <v>2024</v>
+      </c>
       <c r="N10">
+        <v>22.224132521973623</v>
+      </c>
+      <c r="O10">
+        <v>51.308301411534231</v>
+      </c>
+      <c r="R10">
         <v>2024</v>
       </c>
-      <c r="O10" s="14">
+      <c r="S10" s="11">
+        <f t="shared" si="6"/>
         <v>18890.512643677579</v>
       </c>
-      <c r="P10" s="26">
+      <c r="T10" s="20">
+        <f t="shared" si="7"/>
         <v>43612.056199804094</v>
       </c>
-      <c r="Q10" s="29"/>
-      <c r="W10">
+      <c r="U10" s="34"/>
+      <c r="AA10">
         <v>2001</v>
       </c>
-      <c r="X10" s="21">
+      <c r="AB10" s="18">
         <v>27.984999999999999</v>
       </c>
-      <c r="Y10" s="21">
+      <c r="AC10" s="18">
         <v>27.984999999999999</v>
       </c>
-      <c r="Z10" s="21">
+      <c r="AD10" s="18">
         <v>27.984999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2032</v>
       </c>
@@ -3684,56 +3516,67 @@
       <c r="C11">
         <v>198.954028469929</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="1">
         <v>67.492456363636407</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="1">
         <v>403.33153664398401</v>
       </c>
       <c r="F11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>56.59447567260527</v>
       </c>
       <c r="G11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>159.17056032148088</v>
       </c>
       <c r="I11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2031</v>
       </c>
       <c r="J11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>56.59447567260527</v>
       </c>
       <c r="K11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>159.17056032148088</v>
       </c>
+      <c r="M11">
+        <v>2025</v>
+      </c>
       <c r="N11">
+        <v>19.104564444791041</v>
+      </c>
+      <c r="O11">
+        <v>42.464724126126441</v>
+      </c>
+      <c r="R11">
         <v>2025</v>
       </c>
-      <c r="O11" s="14">
-        <v>16238.879778072385</v>
-      </c>
-      <c r="P11" s="26">
-        <v>36095.015507207478</v>
-      </c>
-      <c r="Q11" s="29"/>
-      <c r="W11">
+      <c r="S11" s="11">
+        <f t="shared" si="6"/>
+        <v>16238.879778072383</v>
+      </c>
+      <c r="T11" s="20">
+        <f t="shared" si="7"/>
+        <v>36095.01550720747</v>
+      </c>
+      <c r="U11" s="34"/>
+      <c r="AA11">
         <v>2002</v>
       </c>
-      <c r="X11" s="21">
+      <c r="AB11" s="18">
         <v>42.475999999999999</v>
       </c>
-      <c r="Y11" s="21">
+      <c r="AC11" s="18">
         <v>42.475999999999999</v>
       </c>
-      <c r="Z11" s="21">
+      <c r="AD11" s="18">
         <v>42.475999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2034</v>
       </c>
@@ -3743,56 +3586,67 @@
       <c r="C12">
         <v>223.42721913419001</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="1">
         <v>80.480386363636399</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="1">
         <v>485.16087153802999</v>
       </c>
       <c r="F12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>37.950149863539266</v>
       </c>
       <c r="G12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>120.66485836225978</v>
       </c>
       <c r="I12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2033</v>
       </c>
       <c r="J12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>37.950149863539266</v>
       </c>
       <c r="K12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>120.66485836225978</v>
       </c>
+      <c r="M12">
+        <v>2026</v>
+      </c>
       <c r="N12">
+        <v>19.104564444791041</v>
+      </c>
+      <c r="O12">
+        <v>42.464724126126441</v>
+      </c>
+      <c r="R12">
         <v>2026</v>
       </c>
-      <c r="O12" s="14">
-        <v>16238.879778072385</v>
-      </c>
-      <c r="P12" s="26">
-        <v>36095.015507207478</v>
-      </c>
-      <c r="Q12" s="29"/>
-      <c r="W12">
+      <c r="S12" s="11">
+        <f t="shared" si="6"/>
+        <v>16238.879778072383</v>
+      </c>
+      <c r="T12" s="20">
+        <f t="shared" si="7"/>
+        <v>36095.01550720747</v>
+      </c>
+      <c r="U12" s="34"/>
+      <c r="AA12">
         <v>2003</v>
       </c>
-      <c r="X12" s="21">
+      <c r="AB12" s="18">
         <v>59.744999999999997</v>
       </c>
-      <c r="Y12" s="21">
+      <c r="AC12" s="18">
         <v>59.744999999999997</v>
       </c>
-      <c r="Z12" s="21">
+      <c r="AD12" s="18">
         <v>59.744999999999997</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2036</v>
       </c>
@@ -3802,56 +3656,67 @@
       <c r="C13">
         <v>236.84451085926099</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="1">
         <v>95.322164545454498</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="1">
         <v>524.56542997676604</v>
       </c>
       <c r="F13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>23.595109242592276</v>
       </c>
       <c r="G13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>67.551881970356774</v>
       </c>
       <c r="I13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2035</v>
       </c>
       <c r="J13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>23.595109242592276</v>
       </c>
       <c r="K13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>67.551881970356774</v>
       </c>
+      <c r="M13">
+        <v>2027</v>
+      </c>
       <c r="N13">
+        <v>36.803717115649235</v>
+      </c>
+      <c r="O13">
+        <v>68.348128109348693</v>
+      </c>
+      <c r="R13">
         <v>2027</v>
       </c>
-      <c r="O13" s="14">
-        <v>31283.159548301846</v>
-      </c>
-      <c r="P13" s="26">
-        <v>58095.908892946383</v>
-      </c>
-      <c r="Q13" s="29"/>
-      <c r="W13">
+      <c r="S13" s="11">
+        <f t="shared" si="6"/>
+        <v>31283.15954830185</v>
+      </c>
+      <c r="T13" s="20">
+        <f t="shared" si="7"/>
+        <v>58095.908892946391</v>
+      </c>
+      <c r="U13" s="34"/>
+      <c r="AA13">
         <v>2004</v>
       </c>
-      <c r="X13" s="21">
+      <c r="AB13" s="18">
         <v>94.751999999999995</v>
       </c>
-      <c r="Y13" s="21">
+      <c r="AC13" s="18">
         <v>94.751999999999995</v>
       </c>
-      <c r="Z13" s="21">
+      <c r="AD13" s="18">
         <v>94.751999999999995</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2038</v>
       </c>
@@ -3861,56 +3726,67 @@
       <c r="C14">
         <v>248.95698882873</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="1">
         <v>111.444223636364</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="1">
         <v>582.11597042682502</v>
       </c>
       <c r="F14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>22.698468360309779</v>
       </c>
       <c r="G14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>92.549967585077127</v>
       </c>
       <c r="I14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2037</v>
       </c>
       <c r="J14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>22.698468360309779</v>
       </c>
       <c r="K14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>92.549967585077127</v>
       </c>
+      <c r="M14">
+        <v>2028</v>
+      </c>
       <c r="N14">
+        <v>36.803717115649235</v>
+      </c>
+      <c r="O14">
+        <v>68.348128109348693</v>
+      </c>
+      <c r="R14">
         <v>2028</v>
       </c>
-      <c r="O14" s="14">
-        <v>31283.159548301846</v>
-      </c>
-      <c r="P14" s="26">
-        <v>58095.908892946383</v>
-      </c>
-      <c r="Q14" s="29"/>
-      <c r="W14">
+      <c r="S14" s="11">
+        <f t="shared" si="6"/>
+        <v>31283.15954830185</v>
+      </c>
+      <c r="T14" s="20">
+        <f t="shared" si="7"/>
+        <v>58095.908892946391</v>
+      </c>
+      <c r="U14" s="34"/>
+      <c r="AA14">
         <v>2005</v>
       </c>
-      <c r="X14" s="21">
+      <c r="AB14" s="18">
         <v>96.581173219999997</v>
       </c>
-      <c r="Y14" s="21">
+      <c r="AC14" s="18">
         <v>96.581173219999997</v>
       </c>
-      <c r="Z14" s="21">
+      <c r="AD14" s="18">
         <v>96.581173219999997</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2040</v>
       </c>
@@ -3920,56 +3796,67 @@
       <c r="C15">
         <v>289.64260309998701</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="1">
         <v>127.604308181818</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="1">
         <v>593.87906054333405</v>
       </c>
       <c r="F15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>59.584032552634078</v>
       </c>
       <c r="G15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>33.068110151461141</v>
       </c>
       <c r="I15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2039</v>
       </c>
       <c r="J15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>59.584032552634078</v>
       </c>
       <c r="K15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>33.068110151461141</v>
       </c>
+      <c r="M15">
+        <v>2029</v>
+      </c>
       <c r="N15">
+        <v>51.707378166534909</v>
+      </c>
+      <c r="O15">
+        <v>119.4075594603208</v>
+      </c>
+      <c r="R15">
         <v>2029</v>
       </c>
-      <c r="O15" s="14">
+      <c r="S15" s="11">
+        <f t="shared" si="6"/>
         <v>43951.271441554672</v>
       </c>
-      <c r="P15" s="26">
+      <c r="T15" s="20">
+        <f t="shared" si="7"/>
         <v>101496.42554127268</v>
       </c>
-      <c r="Q15" s="29"/>
-      <c r="W15">
+      <c r="U15" s="34"/>
+      <c r="AA15">
         <v>2006</v>
       </c>
-      <c r="X15" s="21">
+      <c r="AB15" s="18">
         <v>98.21307161</v>
       </c>
-      <c r="Y15" s="21">
+      <c r="AC15" s="18">
         <v>98.21307161</v>
       </c>
-      <c r="Z15" s="21">
+      <c r="AD15" s="18">
         <v>98.21307161</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2042</v>
       </c>
@@ -3979,56 +3866,67 @@
       <c r="C16">
         <v>303.58594854886297</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="1">
         <v>139.236943636364</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="1">
         <v>639.29218521486405</v>
       </c>
       <c r="F16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>23.36514008353878</v>
       </c>
       <c r="G16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>71.832961072989605</v>
       </c>
       <c r="I16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2041</v>
       </c>
       <c r="J16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>23.36514008353878</v>
       </c>
       <c r="K16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>71.832961072989605</v>
       </c>
+      <c r="M16">
+        <v>2030</v>
+      </c>
       <c r="N16">
+        <v>51.707378166534909</v>
+      </c>
+      <c r="O16">
+        <v>119.4075594603208</v>
+      </c>
+      <c r="R16">
         <v>2030</v>
       </c>
-      <c r="O16" s="14">
+      <c r="S16" s="11">
+        <f t="shared" si="6"/>
         <v>43951.271441554672</v>
       </c>
-      <c r="P16" s="26">
+      <c r="T16" s="20">
+        <f t="shared" si="7"/>
         <v>101496.42554127268</v>
       </c>
-      <c r="Q16" s="29"/>
-      <c r="W16">
+      <c r="U16" s="34"/>
+      <c r="AA16">
         <v>2007</v>
       </c>
-      <c r="X16" s="21">
+      <c r="AB16" s="18">
         <v>324.23274839999999</v>
       </c>
-      <c r="Y16" s="21">
+      <c r="AC16" s="18">
         <v>324.23274839999999</v>
       </c>
-      <c r="Z16" s="21">
+      <c r="AD16" s="18">
         <v>324.23274839999999</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2044</v>
       </c>
@@ -4038,56 +3936,67 @@
       <c r="C17">
         <v>336.10154720815598</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="1">
         <v>148.088826363636</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="1">
         <v>682.98325261898503</v>
       </c>
       <c r="F17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>46.985628257080883</v>
       </c>
       <c r="G17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>66.535458625356483</v>
       </c>
       <c r="I17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2043</v>
       </c>
       <c r="J17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>46.985628257080883</v>
       </c>
       <c r="K17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>66.535458625356483</v>
       </c>
+      <c r="M17">
+        <v>2031</v>
+      </c>
       <c r="N17">
+        <v>56.59447567260527</v>
+      </c>
+      <c r="O17">
+        <v>159.17056032148088</v>
+      </c>
+      <c r="R17">
         <v>2031</v>
       </c>
-      <c r="O17" s="14">
+      <c r="S17" s="11">
+        <f t="shared" si="6"/>
         <v>48105.30432171448</v>
       </c>
-      <c r="P17" s="26">
+      <c r="T17" s="20">
+        <f t="shared" si="7"/>
         <v>135294.97627325874</v>
       </c>
-      <c r="Q17" s="29"/>
-      <c r="W17">
+      <c r="U17" s="34"/>
+      <c r="AA17">
         <v>2008</v>
       </c>
-      <c r="X17" s="21">
+      <c r="AB17" s="18">
         <v>314.58510869999998</v>
       </c>
-      <c r="Y17" s="21">
+      <c r="AC17" s="18">
         <v>314.58510869999998</v>
       </c>
-      <c r="Z17" s="21">
+      <c r="AD17" s="18">
         <v>314.58510869999998</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2046</v>
       </c>
@@ -4097,56 +4006,67 @@
       <c r="C18">
         <v>361.99709317474998</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="1">
         <v>155.33214272727301</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18" s="1">
         <v>741.40792082883002</v>
       </c>
       <c r="F18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>38.118722756572225</v>
       </c>
       <c r="G18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>83.919716672799183</v>
       </c>
       <c r="I18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2045</v>
       </c>
       <c r="J18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>38.118722756572225</v>
       </c>
       <c r="K18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>83.919716672799183</v>
       </c>
+      <c r="M18">
+        <v>2032</v>
+      </c>
       <c r="N18">
+        <v>56.59447567260527</v>
+      </c>
+      <c r="O18">
+        <v>159.17056032148088</v>
+      </c>
+      <c r="R18">
         <v>2032</v>
       </c>
-      <c r="O18" s="14">
+      <c r="S18" s="11">
+        <f t="shared" si="6"/>
         <v>48105.30432171448</v>
       </c>
-      <c r="P18" s="26">
+      <c r="T18" s="20">
+        <f t="shared" si="7"/>
         <v>135294.97627325874</v>
       </c>
-      <c r="Q18" s="29"/>
-      <c r="W18">
+      <c r="U18" s="34"/>
+      <c r="AA18">
         <v>2009</v>
       </c>
-      <c r="X18" s="21">
+      <c r="AB18" s="18">
         <v>431.24480390000002</v>
       </c>
-      <c r="Y18" s="21">
+      <c r="AC18" s="18">
         <v>431.24480390000002</v>
       </c>
-      <c r="Z18" s="21">
+      <c r="AD18" s="18">
         <v>431.24480390000002</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2048</v>
       </c>
@@ -4156,56 +4076,67 @@
       <c r="C19">
         <v>399.13920644611602</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="1">
         <v>161.52204727272701</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E19" s="1">
         <v>823.134117188196</v>
       </c>
       <c r="F19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>52.272870252775796</v>
       </c>
       <c r="G19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>113.05295026717518</v>
       </c>
       <c r="I19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2047</v>
       </c>
       <c r="J19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>52.272870252775796</v>
       </c>
       <c r="K19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>113.05295026717518</v>
       </c>
+      <c r="M19">
+        <v>2033</v>
+      </c>
       <c r="N19">
+        <v>37.950149863539266</v>
+      </c>
+      <c r="O19">
+        <v>120.66485836225978</v>
+      </c>
+      <c r="R19">
         <v>2033</v>
       </c>
-      <c r="O19" s="14">
+      <c r="S19" s="11">
+        <f t="shared" si="6"/>
         <v>32257.627384008374</v>
       </c>
-      <c r="P19" s="26">
+      <c r="T19" s="20">
+        <f t="shared" si="7"/>
         <v>102565.12960792081</v>
       </c>
-      <c r="Q19" s="29"/>
-      <c r="W19">
+      <c r="U19" s="34"/>
+      <c r="AA19">
         <v>2010</v>
       </c>
-      <c r="X19" s="21">
+      <c r="AB19" s="18">
         <v>719.84443759999999</v>
       </c>
-      <c r="Y19" s="21">
+      <c r="AC19" s="18">
         <v>719.84443759999999</v>
       </c>
-      <c r="Z19" s="21">
+      <c r="AD19" s="18">
         <v>719.84443759999999</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2050</v>
       </c>
@@ -4215,769 +4146,958 @@
       <c r="C20">
         <v>452.97766085868898</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="1">
         <v>167.21188818181801</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20" s="1">
         <v>907.75283817318802</v>
       </c>
       <c r="F20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>73.621058736344949</v>
       </c>
       <c r="G20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>116.26316228048974</v>
       </c>
       <c r="I20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2049</v>
       </c>
       <c r="J20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>73.621058736344949</v>
       </c>
       <c r="K20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>116.26316228048974</v>
       </c>
+      <c r="M20">
+        <v>2034</v>
+      </c>
       <c r="N20">
+        <v>37.950149863539266</v>
+      </c>
+      <c r="O20">
+        <v>120.66485836225978</v>
+      </c>
+      <c r="R20">
         <v>2034</v>
       </c>
-      <c r="O20" s="14">
+      <c r="S20" s="11">
+        <f t="shared" si="6"/>
         <v>32257.627384008374</v>
       </c>
-      <c r="P20" s="26">
+      <c r="T20" s="20">
+        <f t="shared" si="7"/>
         <v>102565.12960792081</v>
       </c>
-      <c r="Q20" s="29"/>
-      <c r="W20">
+      <c r="U20" s="34"/>
+      <c r="AA20">
         <v>2011</v>
       </c>
-      <c r="X20" s="10">
+      <c r="AB20" s="7">
         <v>1781.377078</v>
       </c>
-      <c r="Y20" s="10">
+      <c r="AC20" s="7">
         <v>1781.377078</v>
       </c>
-      <c r="Z20">
+      <c r="AD20">
         <v>2534.3001088300002</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="M21">
+        <v>2035</v>
+      </c>
       <c r="N21">
+        <v>23.595109242592276</v>
+      </c>
+      <c r="O21">
+        <v>67.551881970356774</v>
+      </c>
+      <c r="R21">
         <v>2035</v>
       </c>
-      <c r="O21" s="14">
+      <c r="S21" s="11">
+        <f t="shared" si="6"/>
         <v>20055.842856203435</v>
       </c>
-      <c r="P21" s="26">
+      <c r="T21" s="20">
+        <f t="shared" si="7"/>
         <v>57419.099674803256</v>
       </c>
-      <c r="Q21" s="29"/>
-      <c r="W21">
+      <c r="U21" s="34"/>
+      <c r="AA21">
         <v>2012</v>
       </c>
-      <c r="X21" s="10">
+      <c r="AB21" s="7">
         <v>3064.1622809999999</v>
       </c>
-      <c r="Y21" s="10">
+      <c r="AC21" s="7">
         <v>3064.1622809999999</v>
       </c>
-      <c r="Z21">
+      <c r="AD21">
         <v>2534.3001088300002</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="M22">
+        <v>2036</v>
+      </c>
       <c r="N22">
+        <v>23.595109242592276</v>
+      </c>
+      <c r="O22">
+        <v>67.551881970356774</v>
+      </c>
+      <c r="R22">
         <v>2036</v>
       </c>
-      <c r="O22" s="14">
+      <c r="S22" s="11">
+        <f t="shared" si="6"/>
         <v>20055.842856203435</v>
       </c>
-      <c r="P22" s="26">
+      <c r="T22" s="20">
+        <f t="shared" si="7"/>
         <v>57419.099674803256</v>
       </c>
-      <c r="Q22" s="29"/>
-      <c r="W22">
+      <c r="U22" s="34"/>
+      <c r="AA22">
         <v>2013</v>
       </c>
-      <c r="X22" s="10">
+      <c r="AB22" s="7">
         <v>4037.4491130000001</v>
       </c>
-      <c r="Y22" s="10">
+      <c r="AC22" s="7">
         <v>4037.4491130000001</v>
       </c>
-      <c r="Z22">
+      <c r="AD22">
         <v>5123.0337317149997</v>
       </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="M23">
+        <v>2037</v>
+      </c>
       <c r="N23">
+        <v>22.698468360309779</v>
+      </c>
+      <c r="O23">
+        <v>92.549967585077127</v>
+      </c>
+      <c r="R23">
         <v>2037</v>
       </c>
-      <c r="O23" s="14">
+      <c r="S23" s="11">
+        <f t="shared" si="6"/>
+        <v>19293.698106263309</v>
+      </c>
+      <c r="T23" s="20">
+        <f t="shared" si="7"/>
+        <v>78667.472447315566</v>
+      </c>
+      <c r="U23" s="34"/>
+      <c r="AA23">
+        <v>2014</v>
+      </c>
+      <c r="AB23" s="7">
+        <v>3722.1994850000001</v>
+      </c>
+      <c r="AC23" s="7">
+        <v>3722.1994850000001</v>
+      </c>
+      <c r="AD23">
+        <v>5123.0337317149997</v>
+      </c>
+    </row>
+    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="M24">
+        <v>2038</v>
+      </c>
+      <c r="N24">
+        <v>22.698468360309779</v>
+      </c>
+      <c r="O24">
+        <v>92.549967585077127</v>
+      </c>
+      <c r="R24">
+        <v>2038</v>
+      </c>
+      <c r="S24" s="11">
+        <f t="shared" si="6"/>
+        <v>19293.698106263309</v>
+      </c>
+      <c r="T24" s="20">
+        <f t="shared" si="7"/>
+        <v>78667.472447315566</v>
+      </c>
+      <c r="U24" s="34"/>
+      <c r="AA24">
+        <v>2015</v>
+      </c>
+      <c r="AB24" s="7">
+        <v>6834.3288130000001</v>
+      </c>
+      <c r="AC24" s="7">
+        <v>6834.3288130000001</v>
+      </c>
+      <c r="AD24">
+        <v>9477.5373098149994</v>
+      </c>
+    </row>
+    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="M25">
+        <v>2039</v>
+      </c>
+      <c r="N25">
+        <v>59.584032552634078</v>
+      </c>
+      <c r="O25">
+        <v>33.068110151461141</v>
+      </c>
+      <c r="R25">
+        <v>2039</v>
+      </c>
+      <c r="S25" s="11">
+        <f t="shared" si="6"/>
+        <v>50646.427669738965</v>
+      </c>
+      <c r="T25" s="20">
+        <f t="shared" si="7"/>
+        <v>28107.893628741971</v>
+      </c>
+      <c r="U25" s="34"/>
+      <c r="AA25">
+        <v>2016</v>
+      </c>
+      <c r="AB25" s="7">
+        <v>12897.665950000001</v>
+      </c>
+      <c r="AC25" s="7">
+        <v>12897.665950000001</v>
+      </c>
+      <c r="AD25">
+        <v>9477.5373098149994</v>
+      </c>
+    </row>
+    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="M26">
+        <v>2040</v>
+      </c>
+      <c r="N26">
+        <v>59.584032552634078</v>
+      </c>
+      <c r="O26">
+        <v>33.068110151461141</v>
+      </c>
+      <c r="R26">
+        <v>2040</v>
+      </c>
+      <c r="S26" s="11">
+        <f t="shared" si="6"/>
+        <v>50646.427669738965</v>
+      </c>
+      <c r="T26" s="20">
+        <f t="shared" si="7"/>
+        <v>28107.893628741971</v>
+      </c>
+      <c r="U26" s="34"/>
+      <c r="AA26">
+        <v>2017</v>
+      </c>
+      <c r="AB26" s="7">
+        <v>9784.5062149999994</v>
+      </c>
+      <c r="AC26" s="7">
+        <v>9784.5062149999994</v>
+      </c>
+      <c r="AD26">
+        <v>9156.7831249049996</v>
+      </c>
+    </row>
+    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="M27">
+        <v>2041</v>
+      </c>
+      <c r="N27">
+        <v>23.36514008353878</v>
+      </c>
+      <c r="O27">
+        <v>71.832961072989605</v>
+      </c>
+      <c r="R27">
+        <v>2041</v>
+      </c>
+      <c r="S27" s="11">
+        <f t="shared" si="6"/>
+        <v>19860.369071007961</v>
+      </c>
+      <c r="T27" s="20">
+        <f t="shared" si="7"/>
+        <v>61058.016912041159</v>
+      </c>
+      <c r="U27" s="34"/>
+      <c r="AA27">
+        <v>2018</v>
+      </c>
+      <c r="AB27" s="7">
+        <v>9352.5294479999993</v>
+      </c>
+      <c r="AC27" s="7">
+        <v>9352.5294479999993</v>
+      </c>
+      <c r="AD27">
+        <v>9156.7831249049996</v>
+      </c>
+    </row>
+    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="M28">
+        <v>2042</v>
+      </c>
+      <c r="N28">
+        <v>23.36514008353878</v>
+      </c>
+      <c r="O28">
+        <v>71.832961072989605</v>
+      </c>
+      <c r="R28">
+        <v>2042</v>
+      </c>
+      <c r="S28" s="11">
+        <f t="shared" si="6"/>
+        <v>19860.369071007961</v>
+      </c>
+      <c r="T28" s="20">
+        <f t="shared" si="7"/>
+        <v>61058.016912041159</v>
+      </c>
+      <c r="U28" s="34"/>
+      <c r="AA28">
+        <v>2019</v>
+      </c>
+      <c r="AB28" s="7">
+        <v>10949.78234</v>
+      </c>
+      <c r="AC28" s="7">
+        <v>10949.78234</v>
+      </c>
+      <c r="AD28">
+        <v>16904.814949799998</v>
+      </c>
+    </row>
+    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="M29">
+        <v>2043</v>
+      </c>
+      <c r="N29">
+        <v>46.985628257080883</v>
+      </c>
+      <c r="O29">
+        <v>66.535458625356483</v>
+      </c>
+      <c r="R29">
+        <v>2043</v>
+      </c>
+      <c r="S29" s="11">
+        <f t="shared" si="6"/>
+        <v>39937.784018518745</v>
+      </c>
+      <c r="T29" s="20">
+        <f t="shared" si="7"/>
+        <v>56555.13983155301</v>
+      </c>
+      <c r="U29" s="34"/>
+      <c r="AA29">
+        <v>2020</v>
+      </c>
+      <c r="AB29">
+        <v>14903.79</v>
+      </c>
+      <c r="AC29">
+        <v>14454.770399725652</v>
+      </c>
+      <c r="AD29">
+        <v>16904.814949799998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="M30">
+        <v>2044</v>
+      </c>
+      <c r="N30">
+        <v>46.985628257080883</v>
+      </c>
+      <c r="O30">
+        <v>66.535458625356483</v>
+      </c>
+      <c r="R30">
+        <v>2044</v>
+      </c>
+      <c r="S30" s="11">
+        <f t="shared" si="6"/>
+        <v>39937.784018518745</v>
+      </c>
+      <c r="T30" s="20">
+        <f t="shared" si="7"/>
+        <v>56555.13983155301</v>
+      </c>
+      <c r="U30" s="34"/>
+      <c r="AA30">
+        <v>2021</v>
+      </c>
+      <c r="AB30">
+        <v>16455.560000000001</v>
+      </c>
+      <c r="AC30">
+        <v>29515.260985639161</v>
+      </c>
+      <c r="AD30">
+        <v>4479.8336675849996</v>
+      </c>
+    </row>
+    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="M31">
+        <v>2045</v>
+      </c>
+      <c r="N31">
+        <v>38.118722756572225</v>
+      </c>
+      <c r="O31">
+        <v>83.919716672799183</v>
+      </c>
+      <c r="R31">
+        <v>2045</v>
+      </c>
+      <c r="S31" s="11">
+        <f t="shared" si="6"/>
+        <v>32400.914343086391</v>
+      </c>
+      <c r="T31" s="20">
+        <f t="shared" si="7"/>
+        <v>71331.759171879297</v>
+      </c>
+      <c r="U31" s="34"/>
+      <c r="AA31">
+        <v>2022</v>
+      </c>
+      <c r="AB31">
+        <v>15227.23</v>
+      </c>
+      <c r="AC31">
+        <v>29515.260985639161</v>
+      </c>
+      <c r="AD31">
+        <v>4479.8336675849996</v>
+      </c>
+    </row>
+    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="M32">
+        <v>2046</v>
+      </c>
+      <c r="N32">
+        <v>38.118722756572225</v>
+      </c>
+      <c r="O32">
+        <v>83.919716672799183</v>
+      </c>
+      <c r="R32">
+        <v>2046</v>
+      </c>
+      <c r="S32" s="11">
+        <f t="shared" si="6"/>
+        <v>32400.914343086391</v>
+      </c>
+      <c r="T32" s="20">
+        <f t="shared" si="7"/>
+        <v>71331.759171879297</v>
+      </c>
+      <c r="U32" s="34"/>
+      <c r="AA32">
+        <v>2023</v>
+      </c>
+      <c r="AB32">
+        <v>15224.02</v>
+      </c>
+      <c r="AC32">
+        <v>18890.512643677579</v>
+      </c>
+      <c r="AD32">
+        <v>13634.589690645</v>
+      </c>
+    </row>
+    <row r="33" spans="13:30" x14ac:dyDescent="0.25">
+      <c r="M33">
+        <v>2047</v>
+      </c>
+      <c r="N33">
+        <v>52.272870252775796</v>
+      </c>
+      <c r="O33">
+        <v>113.05295026717518</v>
+      </c>
+      <c r="R33">
+        <v>2047</v>
+      </c>
+      <c r="S33" s="11">
+        <f t="shared" si="6"/>
+        <v>44431.939714859422</v>
+      </c>
+      <c r="T33" s="20">
+        <f t="shared" si="7"/>
+        <v>96095.007727098899</v>
+      </c>
+      <c r="U33" s="34"/>
+      <c r="AA33">
+        <v>2024</v>
+      </c>
+      <c r="AB33">
+        <v>16634.43</v>
+      </c>
+      <c r="AC33">
+        <v>18890.512643677579</v>
+      </c>
+      <c r="AD33">
+        <v>13634.589690645</v>
+      </c>
+    </row>
+    <row r="34" spans="13:30" x14ac:dyDescent="0.25">
+      <c r="M34">
+        <v>2048</v>
+      </c>
+      <c r="N34">
+        <v>52.272870252775796</v>
+      </c>
+      <c r="O34">
+        <v>113.05295026717518</v>
+      </c>
+      <c r="R34">
+        <v>2048</v>
+      </c>
+      <c r="S34" s="11">
+        <f t="shared" si="6"/>
+        <v>44431.939714859422</v>
+      </c>
+      <c r="T34" s="20">
+        <f t="shared" si="7"/>
+        <v>96095.007727098899</v>
+      </c>
+      <c r="U34" s="34"/>
+      <c r="AA34">
+        <v>2025</v>
+      </c>
+      <c r="AB34">
+        <v>18114.894270000001</v>
+      </c>
+      <c r="AC34">
+        <v>16238.879778072385</v>
+      </c>
+      <c r="AD34">
+        <v>28006.324743929999</v>
+      </c>
+    </row>
+    <row r="35" spans="13:30" x14ac:dyDescent="0.25">
+      <c r="M35">
+        <v>2049</v>
+      </c>
+      <c r="N35">
+        <v>73.621058736344949</v>
+      </c>
+      <c r="O35">
+        <v>116.26316228048974</v>
+      </c>
+      <c r="R35">
+        <v>2049</v>
+      </c>
+      <c r="S35" s="11">
+        <f t="shared" si="6"/>
+        <v>62577.899925893209</v>
+      </c>
+      <c r="T35" s="20">
+        <f t="shared" si="7"/>
+        <v>98823.687938416275</v>
+      </c>
+      <c r="U35" s="34"/>
+      <c r="AA35">
+        <v>2026</v>
+      </c>
+      <c r="AB35">
+        <v>19727.119859999999</v>
+      </c>
+      <c r="AC35">
+        <v>16238.879778072385</v>
+      </c>
+      <c r="AD35">
+        <v>28006.324743929999</v>
+      </c>
+    </row>
+    <row r="36" spans="13:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M36">
+        <v>2050</v>
+      </c>
+      <c r="N36">
+        <v>73.621058736344949</v>
+      </c>
+      <c r="O36">
+        <v>116.26316228048974</v>
+      </c>
+      <c r="R36">
+        <v>2050</v>
+      </c>
+      <c r="S36" s="11">
+        <f t="shared" si="6"/>
+        <v>62577.899925893209</v>
+      </c>
+      <c r="T36" s="20">
+        <f t="shared" si="7"/>
+        <v>98823.687938416275</v>
+      </c>
+      <c r="U36" s="35"/>
+      <c r="AA36">
+        <v>2027</v>
+      </c>
+      <c r="AB36">
+        <v>21482.83353</v>
+      </c>
+      <c r="AC36">
+        <v>31283.159548301846</v>
+      </c>
+      <c r="AD36">
+        <v>26628.140384019898</v>
+      </c>
+    </row>
+    <row r="37" spans="13:30" x14ac:dyDescent="0.25">
+      <c r="AA37">
+        <v>2028</v>
+      </c>
+      <c r="AB37">
+        <v>23394.805710000001</v>
+      </c>
+      <c r="AC37">
+        <v>31283.159548301846</v>
+      </c>
+      <c r="AD37">
+        <v>26628.140384019898</v>
+      </c>
+    </row>
+    <row r="38" spans="13:30" x14ac:dyDescent="0.25">
+      <c r="AA38">
+        <v>2029</v>
+      </c>
+      <c r="AB38">
+        <v>25476.94342</v>
+      </c>
+      <c r="AC38">
+        <v>43951.271441554672</v>
+      </c>
+      <c r="AD38">
+        <v>44459.75121355</v>
+      </c>
+    </row>
+    <row r="39" spans="13:30" x14ac:dyDescent="0.25">
+      <c r="AA39">
+        <v>2030</v>
+      </c>
+      <c r="AB39">
+        <v>27744.391380000001</v>
+      </c>
+      <c r="AC39">
+        <v>43951.271441554672</v>
+      </c>
+      <c r="AD39">
+        <v>44459.75121355</v>
+      </c>
+    </row>
+    <row r="40" spans="13:30" x14ac:dyDescent="0.25">
+      <c r="AA40">
+        <v>2031</v>
+      </c>
+      <c r="AB40">
+        <v>30213.642220000002</v>
+      </c>
+      <c r="AC40">
+        <v>48105.30432171448</v>
+      </c>
+      <c r="AD40">
+        <v>12957.187354395001</v>
+      </c>
+    </row>
+    <row r="41" spans="13:30" x14ac:dyDescent="0.25">
+      <c r="AA41">
+        <v>2032</v>
+      </c>
+      <c r="AB41">
+        <v>32902.656369999997</v>
+      </c>
+      <c r="AC41">
+        <v>48105.30432171448</v>
+      </c>
+      <c r="AD41">
+        <v>12957.187354395001</v>
+      </c>
+    </row>
+    <row r="42" spans="13:30" x14ac:dyDescent="0.25">
+      <c r="AA42">
+        <v>2033</v>
+      </c>
+      <c r="AB42">
+        <v>35830.992789999997</v>
+      </c>
+      <c r="AC42">
+        <v>32257.627384008374</v>
+      </c>
+      <c r="AD42">
+        <v>11610.68853263</v>
+      </c>
+    </row>
+    <row r="43" spans="13:30" x14ac:dyDescent="0.25">
+      <c r="AA43">
+        <v>2034</v>
+      </c>
+      <c r="AB43">
+        <v>39019.951150000001</v>
+      </c>
+      <c r="AC43">
+        <v>32257.627384008374</v>
+      </c>
+      <c r="AD43">
+        <v>11610.68853263</v>
+      </c>
+    </row>
+    <row r="44" spans="13:30" x14ac:dyDescent="0.25">
+      <c r="AA44">
+        <v>2035</v>
+      </c>
+      <c r="AB44">
+        <v>42492.726799999997</v>
+      </c>
+      <c r="AC44">
+        <v>20055.842856203435</v>
+      </c>
+      <c r="AD44">
+        <v>12365.7540896299</v>
+      </c>
+    </row>
+    <row r="45" spans="13:30" x14ac:dyDescent="0.25">
+      <c r="AA45">
+        <v>2036</v>
+      </c>
+      <c r="AB45">
+        <v>46274.579489999996</v>
+      </c>
+      <c r="AC45">
+        <v>20055.842856203435</v>
+      </c>
+      <c r="AD45">
+        <v>12365.7540896299</v>
+      </c>
+    </row>
+    <row r="46" spans="13:30" x14ac:dyDescent="0.25">
+      <c r="AA46">
+        <v>2037</v>
+      </c>
+      <c r="AB46">
+        <v>50393.017059999998</v>
+      </c>
+      <c r="AC46">
         <v>19293.698106263313</v>
       </c>
-      <c r="P23" s="26">
-        <v>78667.472447315566</v>
-      </c>
-      <c r="Q23" s="29"/>
-      <c r="W23">
-        <v>2014</v>
-      </c>
-      <c r="X23" s="10">
-        <v>3722.1994850000001</v>
-      </c>
-      <c r="Y23" s="10">
-        <v>3722.1994850000001</v>
-      </c>
-      <c r="Z23">
-        <v>5123.0337317149997</v>
-      </c>
-    </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="N24">
+      <c r="AD46">
+        <v>21040.884630385</v>
+      </c>
+    </row>
+    <row r="47" spans="13:30" x14ac:dyDescent="0.25">
+      <c r="AA47">
         <v>2038</v>
       </c>
-      <c r="O24" s="14">
+      <c r="AB47">
+        <v>54877.995580000003</v>
+      </c>
+      <c r="AC47">
         <v>19293.698106263313</v>
       </c>
-      <c r="P24" s="26">
-        <v>78667.472447315566</v>
-      </c>
-      <c r="Q24" s="29"/>
-      <c r="W24">
-        <v>2015</v>
-      </c>
-      <c r="X24" s="10">
-        <v>6834.3288130000001</v>
-      </c>
-      <c r="Y24" s="10">
-        <v>6834.3288130000001</v>
-      </c>
-      <c r="Z24">
-        <v>9477.5373098149994</v>
-      </c>
-    </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="N25">
+      <c r="AD47">
+        <v>21040.884630385</v>
+      </c>
+    </row>
+    <row r="48" spans="13:30" x14ac:dyDescent="0.25">
+      <c r="AA48">
         <v>2039</v>
       </c>
-      <c r="O25" s="14">
+      <c r="AB48">
+        <v>59762.137190000001</v>
+      </c>
+      <c r="AC48">
         <v>50646.427669738965</v>
       </c>
-      <c r="P25" s="26">
-        <v>28107.893628741971</v>
-      </c>
-      <c r="Q25" s="29"/>
-      <c r="W25">
-        <v>2016</v>
-      </c>
-      <c r="X25" s="10">
-        <v>12897.665950000001</v>
-      </c>
-      <c r="Y25" s="10">
-        <v>12897.665950000001</v>
-      </c>
-      <c r="Z25">
-        <v>9477.5373098149994</v>
-      </c>
-    </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="N26">
+      <c r="AD48">
+        <v>20625.094014799899</v>
+      </c>
+    </row>
+    <row r="49" spans="27:30" x14ac:dyDescent="0.25">
+      <c r="AA49">
         <v>2040</v>
       </c>
-      <c r="O26" s="14">
+      <c r="AB49">
+        <v>65080.967400000001</v>
+      </c>
+      <c r="AC49">
         <v>50646.427669738965</v>
       </c>
-      <c r="P26" s="26">
-        <v>28107.893628741971</v>
-      </c>
-      <c r="Q26" s="29"/>
-      <c r="W26">
-        <v>2017</v>
-      </c>
-      <c r="X26" s="10">
-        <v>9784.5062149999994</v>
-      </c>
-      <c r="Y26" s="10">
-        <v>9784.5062149999994</v>
-      </c>
-      <c r="Z26">
-        <v>9156.7831249049996</v>
-      </c>
-    </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="N27">
+      <c r="AD49">
+        <v>20625.094014799899</v>
+      </c>
+    </row>
+    <row r="50" spans="27:30" x14ac:dyDescent="0.25">
+      <c r="AA50">
         <v>2041</v>
       </c>
-      <c r="O27" s="14">
+      <c r="AB50">
+        <v>70873.173500000004</v>
+      </c>
+      <c r="AC50">
         <v>19860.369071007961</v>
       </c>
-      <c r="P27" s="26">
-        <v>61058.016912041167</v>
-      </c>
-      <c r="Q27" s="29"/>
-      <c r="W27">
-        <v>2018</v>
-      </c>
-      <c r="X27" s="10">
-        <v>9352.5294479999993</v>
-      </c>
-      <c r="Y27" s="10">
-        <v>9352.5294479999993</v>
-      </c>
-      <c r="Z27">
-        <v>9156.7831249049996</v>
-      </c>
-    </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="N28">
+      <c r="AD50">
+        <v>18778.534320809998</v>
+      </c>
+    </row>
+    <row r="51" spans="27:30" x14ac:dyDescent="0.25">
+      <c r="AA51">
         <v>2042</v>
       </c>
-      <c r="O28" s="14">
+      <c r="AB51">
+        <v>77180.885939999993</v>
+      </c>
+      <c r="AC51">
         <v>19860.369071007961</v>
       </c>
-      <c r="P28" s="26">
-        <v>61058.016912041167</v>
-      </c>
-      <c r="Q28" s="29"/>
-      <c r="W28">
-        <v>2019</v>
-      </c>
-      <c r="X28" s="10">
-        <v>10949.78234</v>
-      </c>
-      <c r="Y28" s="10">
-        <v>10949.78234</v>
-      </c>
-      <c r="Z28">
-        <v>16904.814949799998</v>
-      </c>
-    </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="N29">
+      <c r="AD51">
+        <v>18778.534320809998</v>
+      </c>
+    </row>
+    <row r="52" spans="27:30" x14ac:dyDescent="0.25">
+      <c r="AA52">
         <v>2043</v>
       </c>
-      <c r="O29" s="14">
+      <c r="AB52">
+        <v>84049.984790000002</v>
+      </c>
+      <c r="AC52">
         <v>39937.784018518752</v>
       </c>
-      <c r="P29" s="26">
-        <v>56555.139831553002</v>
-      </c>
-      <c r="Q29" s="29"/>
-      <c r="W29">
-        <v>2020</v>
-      </c>
-      <c r="X29">
-        <v>14903.79</v>
-      </c>
-      <c r="Y29">
-        <v>14454.770399725652</v>
-      </c>
-      <c r="Z29">
-        <v>16904.814949799998</v>
-      </c>
-    </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="N30">
+      <c r="AD52">
+        <v>34424.361313824898</v>
+      </c>
+    </row>
+    <row r="53" spans="27:30" x14ac:dyDescent="0.25">
+      <c r="AA53">
         <v>2044</v>
       </c>
-      <c r="O30" s="14">
+      <c r="AB53">
+        <v>91530.433430000005</v>
+      </c>
+      <c r="AC53">
         <v>39937.784018518752</v>
       </c>
-      <c r="P30" s="26">
-        <v>56555.139831553002</v>
-      </c>
-      <c r="Q30" s="29"/>
-      <c r="W30">
-        <v>2021</v>
-      </c>
-      <c r="X30">
-        <v>16455.560000000001</v>
-      </c>
-      <c r="Y30">
-        <v>29515.260985639161</v>
-      </c>
-      <c r="Z30">
-        <v>4479.8336675849996</v>
-      </c>
-    </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="N31">
+      <c r="AD53">
+        <v>34424.361313824898</v>
+      </c>
+    </row>
+    <row r="54" spans="27:30" x14ac:dyDescent="0.25">
+      <c r="AA54">
         <v>2045</v>
       </c>
-      <c r="O31" s="14">
+      <c r="AB54">
+        <v>99676.642009999996</v>
+      </c>
+      <c r="AC54">
         <v>32400.914343086391</v>
       </c>
-      <c r="P31" s="26">
-        <v>71331.759171879312</v>
-      </c>
-      <c r="Q31" s="29"/>
-      <c r="W31">
-        <v>2022</v>
-      </c>
-      <c r="X31">
-        <v>15227.23</v>
-      </c>
-      <c r="Y31">
-        <v>29515.260985639161</v>
-      </c>
-      <c r="Z31">
-        <v>4479.8336675849996</v>
-      </c>
-    </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="N32">
+      <c r="AD54">
+        <v>26837.672653645001</v>
+      </c>
+    </row>
+    <row r="55" spans="27:30" x14ac:dyDescent="0.25">
+      <c r="AA55">
         <v>2046</v>
       </c>
-      <c r="O32" s="14">
+      <c r="AB55">
+        <v>108547.8631</v>
+      </c>
+      <c r="AC55">
         <v>32400.914343086391</v>
       </c>
-      <c r="P32" s="26">
-        <v>71331.759171879312</v>
-      </c>
-      <c r="Q32" s="29"/>
-      <c r="W32">
-        <v>2023</v>
-      </c>
-      <c r="X32">
-        <v>15224.02</v>
-      </c>
-      <c r="Y32">
-        <v>18890.512643677579</v>
-      </c>
-      <c r="Z32">
-        <v>13634.589690645</v>
-      </c>
-    </row>
-    <row r="33" spans="14:26" x14ac:dyDescent="0.25">
-      <c r="N33">
+      <c r="AD55">
+        <v>26837.672653645001</v>
+      </c>
+    </row>
+    <row r="56" spans="27:30" x14ac:dyDescent="0.25">
+      <c r="AA56">
         <v>2047</v>
       </c>
-      <c r="O33" s="14">
+      <c r="AB56">
+        <v>118208.62300000001</v>
+      </c>
+      <c r="AC56">
         <v>44431.939714859429</v>
       </c>
-      <c r="P33" s="26">
-        <v>96095.007727098899</v>
-      </c>
-      <c r="Q33" s="29"/>
-      <c r="W33">
-        <v>2024</v>
-      </c>
-      <c r="X33">
-        <v>16634.43</v>
-      </c>
-      <c r="Y33">
-        <v>18890.512643677579</v>
-      </c>
-      <c r="Z33">
-        <v>13634.589690645</v>
-      </c>
-    </row>
-    <row r="34" spans="14:26" x14ac:dyDescent="0.25">
-      <c r="N34">
+      <c r="AD56">
+        <v>42306.236152284997</v>
+      </c>
+    </row>
+    <row r="57" spans="27:30" x14ac:dyDescent="0.25">
+      <c r="AA57">
         <v>2048</v>
       </c>
-      <c r="O34" s="14">
+      <c r="AB57">
+        <v>128729.19040000001</v>
+      </c>
+      <c r="AC57">
         <v>44431.939714859429</v>
       </c>
-      <c r="P34" s="26">
-        <v>96095.007727098899</v>
-      </c>
-      <c r="Q34" s="29"/>
-      <c r="W34">
-        <v>2025</v>
-      </c>
-      <c r="X34">
-        <v>18114.894270000001</v>
-      </c>
-      <c r="Y34">
-        <v>16238.879778072385</v>
-      </c>
-      <c r="Z34">
-        <v>28006.324743929999</v>
-      </c>
-    </row>
-    <row r="35" spans="14:26" x14ac:dyDescent="0.25">
-      <c r="N35">
+      <c r="AD57">
+        <v>42306.236152284997</v>
+      </c>
+    </row>
+    <row r="58" spans="27:30" x14ac:dyDescent="0.25">
+      <c r="AA58">
         <v>2049</v>
       </c>
-      <c r="O35" s="14">
+      <c r="AB58">
+        <v>140186.08840000001</v>
+      </c>
+      <c r="AC58">
         <v>62577.899925893202</v>
       </c>
-      <c r="P35" s="26">
-        <v>98823.687938416275</v>
-      </c>
-      <c r="Q35" s="29"/>
-      <c r="W35">
-        <v>2026</v>
-      </c>
-      <c r="X35">
-        <v>19727.119859999999</v>
-      </c>
-      <c r="Y35">
-        <v>16238.879778072385</v>
-      </c>
-      <c r="Z35">
-        <v>28006.324743929999</v>
-      </c>
-    </row>
-    <row r="36" spans="14:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="N36">
+      <c r="AD58">
+        <v>29545.326875395</v>
+      </c>
+    </row>
+    <row r="59" spans="27:30" x14ac:dyDescent="0.25">
+      <c r="AA59">
         <v>2050</v>
       </c>
-      <c r="O36" s="18">
+      <c r="AB59">
+        <v>152662.6502</v>
+      </c>
+      <c r="AC59">
         <v>62577.899925893202</v>
       </c>
-      <c r="P36" s="27">
-        <v>98823.687938416275</v>
-      </c>
-      <c r="Q36" s="30"/>
-      <c r="W36">
-        <v>2027</v>
-      </c>
-      <c r="X36">
-        <v>21482.83353</v>
-      </c>
-      <c r="Y36">
-        <v>31283.159548301846</v>
-      </c>
-      <c r="Z36">
-        <v>26628.140384019898</v>
-      </c>
-    </row>
-    <row r="37" spans="14:26" x14ac:dyDescent="0.25">
-      <c r="W37">
-        <v>2028</v>
-      </c>
-      <c r="X37">
-        <v>23394.805710000001</v>
-      </c>
-      <c r="Y37">
-        <v>31283.159548301846</v>
-      </c>
-      <c r="Z37">
-        <v>26628.140384019898</v>
-      </c>
-    </row>
-    <row r="38" spans="14:26" x14ac:dyDescent="0.25">
-      <c r="W38">
-        <v>2029</v>
-      </c>
-      <c r="X38">
-        <v>25476.94342</v>
-      </c>
-      <c r="Y38">
-        <v>43951.271441554672</v>
-      </c>
-      <c r="Z38">
-        <v>44459.75121355</v>
-      </c>
-    </row>
-    <row r="39" spans="14:26" x14ac:dyDescent="0.25">
-      <c r="W39">
-        <v>2030</v>
-      </c>
-      <c r="X39">
-        <v>27744.391380000001</v>
-      </c>
-      <c r="Y39">
-        <v>43951.271441554672</v>
-      </c>
-      <c r="Z39">
-        <v>44459.75121355</v>
-      </c>
-    </row>
-    <row r="40" spans="14:26" x14ac:dyDescent="0.25">
-      <c r="W40">
-        <v>2031</v>
-      </c>
-      <c r="X40">
-        <v>30213.642220000002</v>
-      </c>
-      <c r="Y40">
-        <v>48105.30432171448</v>
-      </c>
-      <c r="Z40">
-        <v>12957.187354395001</v>
-      </c>
-    </row>
-    <row r="41" spans="14:26" x14ac:dyDescent="0.25">
-      <c r="W41">
-        <v>2032</v>
-      </c>
-      <c r="X41">
-        <v>32902.656369999997</v>
-      </c>
-      <c r="Y41">
-        <v>48105.30432171448</v>
-      </c>
-      <c r="Z41">
-        <v>12957.187354395001</v>
-      </c>
-    </row>
-    <row r="42" spans="14:26" x14ac:dyDescent="0.25">
-      <c r="W42">
-        <v>2033</v>
-      </c>
-      <c r="X42">
-        <v>35830.992789999997</v>
-      </c>
-      <c r="Y42">
-        <v>32257.627384008374</v>
-      </c>
-      <c r="Z42">
-        <v>11610.68853263</v>
-      </c>
-    </row>
-    <row r="43" spans="14:26" x14ac:dyDescent="0.25">
-      <c r="W43">
-        <v>2034</v>
-      </c>
-      <c r="X43">
-        <v>39019.951150000001</v>
-      </c>
-      <c r="Y43">
-        <v>32257.627384008374</v>
-      </c>
-      <c r="Z43">
-        <v>11610.68853263</v>
-      </c>
-    </row>
-    <row r="44" spans="14:26" x14ac:dyDescent="0.25">
-      <c r="W44">
-        <v>2035</v>
-      </c>
-      <c r="X44">
-        <v>42492.726799999997</v>
-      </c>
-      <c r="Y44">
-        <v>20055.842856203435</v>
-      </c>
-      <c r="Z44">
-        <v>12365.7540896299</v>
-      </c>
-    </row>
-    <row r="45" spans="14:26" x14ac:dyDescent="0.25">
-      <c r="W45">
-        <v>2036</v>
-      </c>
-      <c r="X45">
-        <v>46274.579489999996</v>
-      </c>
-      <c r="Y45">
-        <v>20055.842856203435</v>
-      </c>
-      <c r="Z45">
-        <v>12365.7540896299</v>
-      </c>
-    </row>
-    <row r="46" spans="14:26" x14ac:dyDescent="0.25">
-      <c r="W46">
-        <v>2037</v>
-      </c>
-      <c r="X46">
-        <v>50393.017059999998</v>
-      </c>
-      <c r="Y46">
-        <v>19293.698106263313</v>
-      </c>
-      <c r="Z46">
-        <v>21040.884630385</v>
-      </c>
-    </row>
-    <row r="47" spans="14:26" x14ac:dyDescent="0.25">
-      <c r="W47">
-        <v>2038</v>
-      </c>
-      <c r="X47">
-        <v>54877.995580000003</v>
-      </c>
-      <c r="Y47">
-        <v>19293.698106263313</v>
-      </c>
-      <c r="Z47">
-        <v>21040.884630385</v>
-      </c>
-    </row>
-    <row r="48" spans="14:26" x14ac:dyDescent="0.25">
-      <c r="W48">
-        <v>2039</v>
-      </c>
-      <c r="X48">
-        <v>59762.137190000001</v>
-      </c>
-      <c r="Y48">
-        <v>50646.427669738965</v>
-      </c>
-      <c r="Z48">
-        <v>20625.094014799899</v>
-      </c>
-    </row>
-    <row r="49" spans="23:26" x14ac:dyDescent="0.25">
-      <c r="W49">
-        <v>2040</v>
-      </c>
-      <c r="X49">
-        <v>65080.967400000001</v>
-      </c>
-      <c r="Y49">
-        <v>50646.427669738965</v>
-      </c>
-      <c r="Z49">
-        <v>20625.094014799899</v>
-      </c>
-    </row>
-    <row r="50" spans="23:26" x14ac:dyDescent="0.25">
-      <c r="W50">
-        <v>2041</v>
-      </c>
-      <c r="X50">
-        <v>70873.173500000004</v>
-      </c>
-      <c r="Y50">
-        <v>19860.369071007961</v>
-      </c>
-      <c r="Z50">
-        <v>18778.534320809998</v>
-      </c>
-    </row>
-    <row r="51" spans="23:26" x14ac:dyDescent="0.25">
-      <c r="W51">
-        <v>2042</v>
-      </c>
-      <c r="X51">
-        <v>77180.885939999993</v>
-      </c>
-      <c r="Y51">
-        <v>19860.369071007961</v>
-      </c>
-      <c r="Z51">
-        <v>18778.534320809998</v>
-      </c>
-    </row>
-    <row r="52" spans="23:26" x14ac:dyDescent="0.25">
-      <c r="W52">
-        <v>2043</v>
-      </c>
-      <c r="X52">
-        <v>84049.984790000002</v>
-      </c>
-      <c r="Y52">
-        <v>39937.784018518752</v>
-      </c>
-      <c r="Z52">
-        <v>34424.361313824898</v>
-      </c>
-    </row>
-    <row r="53" spans="23:26" x14ac:dyDescent="0.25">
-      <c r="W53">
-        <v>2044</v>
-      </c>
-      <c r="X53">
-        <v>91530.433430000005</v>
-      </c>
-      <c r="Y53">
-        <v>39937.784018518752</v>
-      </c>
-      <c r="Z53">
-        <v>34424.361313824898</v>
-      </c>
-    </row>
-    <row r="54" spans="23:26" x14ac:dyDescent="0.25">
-      <c r="W54">
-        <v>2045</v>
-      </c>
-      <c r="X54">
-        <v>99676.642009999996</v>
-      </c>
-      <c r="Y54">
-        <v>32400.914343086391</v>
-      </c>
-      <c r="Z54">
-        <v>26837.672653645001</v>
-      </c>
-    </row>
-    <row r="55" spans="23:26" x14ac:dyDescent="0.25">
-      <c r="W55">
-        <v>2046</v>
-      </c>
-      <c r="X55">
-        <v>108547.8631</v>
-      </c>
-      <c r="Y55">
-        <v>32400.914343086391</v>
-      </c>
-      <c r="Z55">
-        <v>26837.672653645001</v>
-      </c>
-    </row>
-    <row r="56" spans="23:26" x14ac:dyDescent="0.25">
-      <c r="W56">
-        <v>2047</v>
-      </c>
-      <c r="X56">
-        <v>118208.62300000001</v>
-      </c>
-      <c r="Y56">
-        <v>44431.939714859429</v>
-      </c>
-      <c r="Z56">
-        <v>42306.236152284997</v>
-      </c>
-    </row>
-    <row r="57" spans="23:26" x14ac:dyDescent="0.25">
-      <c r="W57">
-        <v>2048</v>
-      </c>
-      <c r="X57">
-        <v>128729.19040000001</v>
-      </c>
-      <c r="Y57">
-        <v>44431.939714859429</v>
-      </c>
-      <c r="Z57">
-        <v>42306.236152284997</v>
-      </c>
-    </row>
-    <row r="58" spans="23:26" x14ac:dyDescent="0.25">
-      <c r="W58">
-        <v>2049</v>
-      </c>
-      <c r="X58">
-        <v>140186.08840000001</v>
-      </c>
-      <c r="Y58">
-        <v>62577.899925893202</v>
-      </c>
-      <c r="Z58">
+      <c r="AD59">
         <v>29545.326875395</v>
       </c>
     </row>
-    <row r="59" spans="23:26" x14ac:dyDescent="0.25">
-      <c r="W59">
-        <v>2050</v>
-      </c>
-      <c r="X59">
-        <v>152662.6502</v>
-      </c>
-      <c r="Y59">
-        <v>62577.899925893202</v>
-      </c>
-      <c r="Z59">
-        <v>29545.326875395</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="N4:P36">
-    <sortCondition ref="N4:N36"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="M4:O36">
+    <sortCondition ref="M4:M36"/>
   </sortState>
-  <mergeCells count="3">
-    <mergeCell ref="N1:P1"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="Q6:Q36"/>
+  <mergeCells count="5">
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="U6:U36"/>
+    <mergeCell ref="I2:K2"/>
+    <mergeCell ref="M2:O2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>